<commit_message>
Added login functionality. Began work on sign up page and functionality.
</commit_message>
<xml_diff>
--- a/ExcelUtility/data/TestData.xlsx
+++ b/ExcelUtility/data/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\ExcelUtility\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nino Hana\Documents\GitHub\TeamBread\ExcelUtility\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE530B28-6832-4F92-BC97-727E07182286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1511011-13DE-417F-B852-13F4D6032369}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35430" yWindow="1380" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Student Number</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Daniel</t>
   </si>
   <si>
@@ -52,6 +49,69 @@
   </si>
   <si>
     <t>mpence@usa.com</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>STUDENT</t>
+  </si>
+  <si>
+    <t>PROFESSOR</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>password12</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t>iamthesupreme</t>
+  </si>
+  <si>
+    <t>nhana@eorzea.ca</t>
+  </si>
+  <si>
+    <t>bloodforthelilies</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Nino</t>
+  </si>
+  <si>
+    <t>Saki</t>
+  </si>
+  <si>
+    <t>Yaki</t>
+  </si>
+  <si>
+    <t>Hana</t>
+  </si>
+  <si>
+    <t>Pence</t>
+  </si>
+  <si>
+    <t>Trump</t>
+  </si>
+  <si>
+    <t>Kolocka</t>
+  </si>
+  <si>
+    <t>beefy@sfu.ca</t>
+  </si>
+  <si>
+    <t>100percentorangejuice</t>
   </si>
 </sst>
 </file>
@@ -380,68 +440,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>301333797</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>301333797</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>301333333</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>301333333</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>3012222222</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>3012222222</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>1514131211</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>384920312</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{C768D290-0AB0-433F-AF88-120B739280A9}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{FC78AA51-F642-465F-A2E1-4FF79E16A494}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{89601D26-2E97-4054-B120-3FF157269ACD}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{C768D290-0AB0-433F-AF88-120B739280A9}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{FC78AA51-F642-465F-A2E1-4FF79E16A494}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{89601D26-2E97-4054-B120-3FF157269ACD}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{610E70AB-E78F-4863-BB21-C699E6BBACA6}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{07D7DE8E-1E2D-45D6-8990-4FAA2751BB9F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>